<commit_message>
vault backup: 2025-03-04 12:01:04
</commit_message>
<xml_diff>
--- a/Economics/Dissertation/Dissertation Sheets.xlsx
+++ b/Economics/Dissertation/Dissertation Sheets.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Economics\Dissertation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OWNER\Documents\Notes\PPE\Economics\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F05E4BCA-525F-4E8B-879E-AB934EDB5E4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150EEEC0-39AC-4098-A729-EF58A8E81D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E7F3A71-BFC8-4E5A-9B94-DE35856B8CBC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{5E7F3A71-BFC8-4E5A-9B94-DE35856B8CBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Median Comp and Productivity" sheetId="1" r:id="rId1"/>
@@ -143,7 +143,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="###,###,##0.00"/>
+    <numFmt numFmtId="165" formatCode="###,###,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -231,10 +231,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -293,12 +293,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
-              <a:t>Median</a:t>
-            </a:r>
-            <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> Wages</a:t>
+              <a:t>Evolution of median wages and labour productivity in the UK, 1997=100</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -342,15 +338,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Median Comp and Productivity'!$A$10</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Median Wage Index 1997=100</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Median wages adjusted using CPI</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -527,15 +515,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Median Comp and Productivity'!$A$11</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>OpH Index 1997=100</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Productivity adjusted using Output Price Deflator</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -769,6 +749,8 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="2"/>
+        <c:tickMarkSkip val="1"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
@@ -1471,16 +1453,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>100011</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>556253</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>5937</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>344938</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>164629</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1827,16 +1809,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34019E1C-637C-4A65-AF2C-5C3EB48F59C7}">
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="25.1796875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1910,7 +1892,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -1984,7 +1966,7 @@
         <v>1.0780000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -2058,7 +2040,7 @@
         <v>13.28</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -2132,7 +2114,7 @@
         <v>33.014206715486473</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>25</v>
       </c>
@@ -2229,7 +2211,7 @@
         <v>12.319109461966603</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2303,7 +2285,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
@@ -2400,7 +2382,7 @@
         <v>107.92927702267183</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>29</v>
       </c>
@@ -2497,7 +2479,7 @@
         <v>1.0792927702267183</v>
       </c>
     </row>
-    <row r="9" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>30</v>
       </c>
@@ -2594,7 +2576,7 @@
         <v>30.588740725606311</v>
       </c>
     </row>
-    <row r="10" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>31</v>
       </c>
@@ -2603,7 +2585,7 @@
         <v>100</v>
       </c>
       <c r="C10">
-        <f t="shared" ref="C10:X11" si="4">C5*100/$B5</f>
+        <f t="shared" ref="C10:X10" si="4">C5*100/$B5</f>
         <v>102.49352383071371</v>
       </c>
       <c r="D10">
@@ -2691,7 +2673,7 @@
         <v>122.1456256412813</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>

</xml_diff>